<commit_message>
Updated purchase list, added Ellison time card
</commit_message>
<xml_diff>
--- a/Technical/Hardware/purchase_list.xlsx
+++ b/Technical/Hardware/purchase_list.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Hardware Name</t>
   </si>
@@ -69,18 +70,12 @@
     <t>https://www.sparkfun.com/products/13680</t>
   </si>
   <si>
-    <t>Ultrasonic Range Finder</t>
-  </si>
-  <si>
     <t>Obstacle avoidance prototyping</t>
   </si>
   <si>
     <t>10-20(?)</t>
   </si>
   <si>
-    <t>https://www.sparkfun.com/products/639</t>
-  </si>
-  <si>
     <t>Range finder computer interfacing</t>
   </si>
   <si>
@@ -94,18 +89,67 @@
   </si>
   <si>
     <t>Teensy board</t>
+  </si>
+  <si>
+    <t>Controls processing</t>
+  </si>
+  <si>
+    <t>http://www.hardkernel.com/main/products/prdt_info.php?g_code=G143452239825</t>
+  </si>
+  <si>
+    <t>Ultrasonic Range Finder (narrow beam)</t>
+  </si>
+  <si>
+    <t>Ultrasonic Range Finder (wide beam)</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9491</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9495</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>Prototyping</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/116</t>
+  </si>
+  <si>
+    <t>Breadboard</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/12615</t>
+  </si>
+  <si>
+    <t>Jumpers</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9140</t>
+  </si>
+  <si>
+    <t>Wire Kit</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/124</t>
+  </si>
+  <si>
+    <t>ODROID XU4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -117,6 +161,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,20 +211,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -504,15 +558,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="70" bestFit="1" customWidth="1"/>
@@ -582,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F7" si="0">C3*E3</f>
+        <f t="shared" ref="F3:F8" si="0">C3*E3</f>
         <v>170</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -615,105 +669,187 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="3">
+        <v>49.95</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="3">
-        <v>25.95</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="0"/>
-        <v>25.95</v>
+        <f>C5*E5</f>
+        <v>49.95</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3">
-        <v>19.95</v>
+        <v>49.95</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
+        <v>49.95</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
         <v>19.95</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>39.9</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="C8" s="3">
+        <v>75</v>
+      </c>
+      <c r="D8" s="2">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1.5</v>
+      </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7">
+        <f>C9*E9</f>
+        <v>7.5</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7">
+        <v>5.95</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <f>C10*E10</f>
+        <v>5.95</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7">
+        <v>3.95</v>
+      </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <f>C11*E11</f>
+        <v>3.95</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7">
+        <v>6.95</v>
+      </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
+        <f>C12*E12</f>
+        <v>6.95</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2"/>
@@ -751,23 +887,51 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="5:6">
-      <c r="E17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="3">
-        <f>SUM(F2:F16)</f>
-        <v>521.34</v>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="E18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3">
+        <f>SUM(F2:F17)</f>
+        <v>714.59000000000015</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="G4" r:id="rId2"/>
-    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="G9" r:id="rId3"/>
+    <hyperlink ref="G10" r:id="rId4"/>
+    <hyperlink ref="G11" r:id="rId5"/>
+    <hyperlink ref="G12" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>